<commit_message>
Add code update account
</commit_message>
<xml_diff>
--- a/document/doc.xlsx
+++ b/document/doc.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="101">
   <si>
     <t>No.</t>
   </si>
@@ -246,9 +246,6 @@
   </si>
   <si>
     <t>Phase 1( 1 tháng ): HTML với thực hiện hành đông cơ bản của trang</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>?</t>
@@ -796,7 +793,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,23 +822,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,29 +855,47 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2713,7 +2716,7 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E6"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,14 +2755,14 @@
         <v>5</v>
       </c>
       <c r="G1" s="3"/>
-      <c r="I1" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="33" t="s">
+      <c r="I1" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>70</v>
       </c>
       <c r="K1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2779,14 +2782,14 @@
       <c r="F2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="32"/>
+      <c r="G2" s="26"/>
       <c r="I2">
         <v>4</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="54"/>
+      <c r="K2" s="41"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -2800,7 +2803,7 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>10</v>
@@ -2809,71 +2812,75 @@
       <c r="I3">
         <v>2</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K3" s="54">
+      <c r="K3" s="41">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="3"/>
       <c r="I4">
         <v>2</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="54"/>
+      <c r="K4" s="41">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="3"/>
       <c r="I5">
         <v>2</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="54"/>
-      <c r="L5" s="30"/>
+      <c r="K5" s="41">
+        <v>4</v>
+      </c>
+      <c r="L5" s="24"/>
       <c r="M5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+      <c r="A6" s="22">
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -2884,7 +2891,7 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="15" t="s">
         <v>10</v>
@@ -2893,11 +2900,11 @@
       <c r="I6">
         <v>2</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="54"/>
-      <c r="L6" s="31"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="25"/>
       <c r="M6" t="s">
         <v>69</v>
       </c>
@@ -2914,7 +2921,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>10</v>
@@ -2923,13 +2930,13 @@
       <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="54">
+      <c r="K7" s="41">
         <v>6</v>
       </c>
-      <c r="L7" s="21"/>
+      <c r="L7" s="18"/>
       <c r="M7" t="s">
         <v>66</v>
       </c>
@@ -2946,7 +2953,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>10</v>
@@ -2955,10 +2962,10 @@
       <c r="I8">
         <v>2</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J8" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="54">
+      <c r="K8" s="41">
         <v>6</v>
       </c>
       <c r="M8" t="s">
@@ -2977,7 +2984,7 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>23</v>
@@ -2986,72 +2993,72 @@
       <c r="I9">
         <v>2</v>
       </c>
-      <c r="J9" s="33" t="s">
+      <c r="J9" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K9" s="54">
-        <v>6</v>
-      </c>
-      <c r="L9" s="32"/>
+      <c r="K9" s="41">
+        <v>8</v>
+      </c>
+      <c r="L9" s="26"/>
       <c r="M9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="20" t="s">
+      <c r="F10" s="19"/>
+      <c r="G10" s="17" t="s">
         <v>62</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="54">
+      <c r="K10" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="20"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="17"/>
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11" s="33" t="s">
+      <c r="J11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="54">
+      <c r="K11" s="41">
         <v>1</v>
       </c>
       <c r="L11" t="s">
@@ -3059,94 +3066,94 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="20"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="17"/>
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="54">
+      <c r="K12" s="41">
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="20"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="17"/>
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="54">
+      <c r="K13" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="20"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="17"/>
       <c r="I14">
         <v>1</v>
       </c>
-      <c r="J14" s="33" t="s">
+      <c r="J14" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="54">
+      <c r="K14" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="22">
         <v>14</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -3156,19 +3163,21 @@
         <v>36</v>
       </c>
       <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="F15" s="12"/>
       <c r="G15" s="3"/>
       <c r="I15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J15" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="54"/>
+      <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="A16" s="22">
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -3178,19 +3187,21 @@
         <v>38</v>
       </c>
       <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="F16" s="12"/>
       <c r="G16" s="3"/>
       <c r="I16" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="54"/>
+      <c r="K16" s="41"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="22">
         <v>16</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -3200,133 +3211,135 @@
         <v>40</v>
       </c>
       <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>100</v>
+      </c>
       <c r="F17" s="12"/>
       <c r="G17" s="3"/>
       <c r="I17">
         <v>3</v>
       </c>
-      <c r="J17" s="33" t="s">
+      <c r="J17" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="54"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="48">
+      <c r="A18" s="54">
         <v>17</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="16" t="s">
+      <c r="D18" s="57"/>
+      <c r="E18" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="47"/>
+      <c r="G18" s="53"/>
       <c r="I18">
         <v>8</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="J18" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="54"/>
+      <c r="K18" s="41"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="17" t="s">
+      <c r="A19" s="55"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="47"/>
+      <c r="G19" s="53"/>
       <c r="I19">
         <v>8</v>
       </c>
-      <c r="J19" s="33" t="s">
+      <c r="J19" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="54"/>
+      <c r="K19" s="41"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="18" t="s">
+      <c r="A20" s="56"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="47"/>
+      <c r="G20" s="53"/>
       <c r="I20">
         <v>8</v>
       </c>
-      <c r="J20" s="33" t="s">
+      <c r="J20" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="54"/>
-    </row>
-    <row r="21" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="K20" s="41"/>
+    </row>
+    <row r="21" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="46">
         <v>18</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F21" s="24" t="s">
+      <c r="D21" s="48"/>
+      <c r="E21" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="G21" s="32"/>
-      <c r="I21" s="29">
+      <c r="G21" s="26"/>
+      <c r="I21" s="23">
         <v>6</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="K21" s="54"/>
-    </row>
-    <row r="22" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="K21" s="41"/>
+    </row>
+    <row r="22" spans="1:11" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="46">
         <v>19</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="D22" s="51"/>
+      <c r="E22" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="I22" s="29">
+      <c r="G22" s="26"/>
+      <c r="I22" s="23">
         <v>5</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="54"/>
+      <c r="K22" s="41"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
+      <c r="A23" s="22">
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -3336,21 +3349,21 @@
         <v>53</v>
       </c>
       <c r="D23" s="12"/>
-      <c r="E23" s="12" t="s">
-        <v>71</v>
+      <c r="E23" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="3"/>
-      <c r="I23" s="29">
+      <c r="I23" s="23">
         <v>8</v>
       </c>
-      <c r="J23" s="33" t="s">
+      <c r="J23" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="54"/>
+      <c r="K23" s="41"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="28">
+      <c r="A24" s="22">
         <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -3360,21 +3373,21 @@
         <v>55</v>
       </c>
       <c r="D24" s="12"/>
-      <c r="E24" s="12" t="s">
-        <v>71</v>
+      <c r="E24" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="3"/>
-      <c r="I24" s="29">
+      <c r="I24" s="23">
         <v>3</v>
       </c>
-      <c r="J24" s="34" t="s">
+      <c r="J24" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="K24" s="54"/>
+      <c r="K24" s="41"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="A25" s="22">
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -3384,42 +3397,44 @@
         <v>57</v>
       </c>
       <c r="D25" s="12"/>
-      <c r="E25" s="12" t="s">
-        <v>71</v>
+      <c r="E25" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="3"/>
       <c r="I25">
         <v>7</v>
       </c>
-      <c r="J25" s="34" t="s">
+      <c r="J25" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="K25" s="54"/>
+      <c r="K25" s="41"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+      <c r="A26" s="46">
         <v>23</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="11" t="s">
+      <c r="D26" s="51"/>
+      <c r="E26" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="52" t="s">
         <v>60</v>
       </c>
       <c r="G26" s="3"/>
       <c r="I26" t="s">
         <v>73</v>
       </c>
-      <c r="J26" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="54"/>
+      <c r="J26" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" s="41"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
@@ -3429,10 +3444,10 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="3"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="54">
+      <c r="J27" s="27"/>
+      <c r="K27" s="41">
         <f>SUM(K2:K26)</f>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3443,8 +3458,8 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="3"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="55"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="42"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -3454,8 +3469,8 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="3"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="55"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="42"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
@@ -3465,7 +3480,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="3"/>
-      <c r="J30" s="33"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
@@ -3475,11 +3490,11 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="3"/>
-      <c r="J31" s="33"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3507,7 +3522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J4:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
@@ -3518,20 +3533,20 @@
   <sheetData>
     <row r="4" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
-        <v>80</v>
-      </c>
-      <c r="K6" s="37" t="s">
         <v>79</v>
       </c>
+      <c r="K6" s="31" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="8" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="J8" s="36" t="s">
-        <v>78</v>
+      <c r="J8" s="30" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3552,158 +3567,158 @@
   <sheetData>
     <row r="2" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="8:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="8:12" x14ac:dyDescent="0.25">
       <c r="K11" t="s">
-        <v>94</v>
-      </c>
-      <c r="L11" s="37" t="s">
         <v>93</v>
       </c>
+      <c r="L11" s="31" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="K12" s="36" t="s">
-        <v>92</v>
+      <c r="K12" s="30" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="36" t="s">
-        <v>99</v>
+      <c r="K25" s="30" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="10:11" x14ac:dyDescent="0.25">
-      <c r="K26" s="36" t="s">
-        <v>90</v>
+      <c r="K26" s="30" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="46"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="44"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="38"/>
       <c r="J41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="43"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="41"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="35"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="43"/>
-      <c r="C43" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="41"/>
-      <c r="K43" s="36" t="s">
+      <c r="B43" s="37"/>
+      <c r="C43" s="36" t="s">
         <v>87</v>
       </c>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="K43" s="30" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="43"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="41"/>
-      <c r="K44" s="36" t="s">
-        <v>86</v>
+      <c r="B44" s="37"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="K44" s="30" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="43"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="41"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="35"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="43"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="41"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="43"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="42"/>
-      <c r="F47" s="42"/>
-      <c r="G47" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H47" s="41"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H47" s="35"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="40"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="38"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="32"/>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N54" s="36" t="s">
-        <v>83</v>
+      <c r="N54" s="30" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="N55" s="36" t="s">
-        <v>82</v>
+      <c r="N55" s="30" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>